<commit_message>
customizing the update and delete function
</commit_message>
<xml_diff>
--- a/support docs/WalletTransactionsMockData.xlsx
+++ b/support docs/WalletTransactionsMockData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\74184\Documents\workspace-spring-tool-suite-4-4.14.1.RELEASE\application ideas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\74184\Documents\workspace-spring-tool-suite-4-4.14.1.RELEASE\PersonalFinancing\support docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD889549-EDDA-4453-A8F5-88170808434D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F4F981-078B-41E5-9755-1517ED03655C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FEBD76D-0568-47E0-967A-0A217D5DCFDE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (</t>
+  </si>
+  <si>
+    <t>insert into Wallets (name,description,balances, created_date,update_date) VALUES (</t>
+  </si>
+  <si>
+    <t>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values (</t>
   </si>
 </sst>
 </file>
@@ -540,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD99DCA-BC70-4422-9213-876D15C92D76}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +562,7 @@
     <col min="8" max="8" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="236.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="232.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26.85546875" customWidth="1"/>
   </cols>
@@ -591,6 +598,9 @@
       <c r="K1" t="s">
         <v>48</v>
       </c>
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -628,6 +638,10 @@
         <f>_xlfn.CONCAT($K$1,A2,",'",B2,"','",C2,"','",D2,"',",E2,",",F2,",",H2,",",I2,",",J2,");")</f>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (1,'McDonald','eating big mac','Eatout',-1.59,3,PARSEDATETIME('01/23/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L2" t="str">
+        <f>_xlfn.CONCAT($L$1,"'",B2,"','",C2,"','",D2,"',",E2,",",F2,",",H2,",",I2,",",J2,");")</f>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('McDonald','eating big mac','Eatout',-1.59,3,PARSEDATETIME('01/23/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -666,6 +680,10 @@
         <f t="shared" ref="K3:K14" si="1">_xlfn.CONCAT($K$1,A3,",'",B3,"','",C3,"','",D3,"',",E3,",",F3,",",H3,",",I3,",",J3,");")</f>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (2,'Game Store','buying Nintendo','entertainment ',-150,3,PARSEDATETIME('02/14/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L14" si="2">_xlfn.CONCAT($L$1,"'",B3,"','",C3,"','",D3,"',",E3,",",F3,",",H3,",",I3,",",J3,");")</f>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('Game Store','buying Nintendo','entertainment ',-150,3,PARSEDATETIME('02/14/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -704,6 +722,10 @@
         <f t="shared" si="1"/>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (3,'Transfer','to CO checking','transfer',-500,2,PARSEDATETIME('01/30/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L4" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('Transfer','to CO checking','transfer',-500,2,PARSEDATETIME('01/30/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -742,6 +764,10 @@
         <f t="shared" si="1"/>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (4,'Transfer','from CO saving','transfer',500,1,PARSEDATETIME('01/30/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L5" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('Transfer','from CO saving','transfer',500,1,PARSEDATETIME('01/30/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -780,6 +806,10 @@
         <f t="shared" si="1"/>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (5,'Employer ','paydate','income',2000,2,PARSEDATETIME('01/01/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L6" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('Employer ','paydate','income',2000,2,PARSEDATETIME('01/01/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -818,6 +848,10 @@
         <f t="shared" si="1"/>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (6,'withdraw','take some cash from the checking CO','withdraw',500,6,PARSEDATETIME('01/05/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L7" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('withdraw','take some cash from the checking CO','withdraw',500,6,PARSEDATETIME('01/05/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -856,6 +890,10 @@
         <f t="shared" si="1"/>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (7,'withdraw','take some cash from the checking CO','withdraw',-500,1,PARSEDATETIME('01/05/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L8" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('withdraw','take some cash from the checking CO','withdraw',-500,1,PARSEDATETIME('01/05/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -894,6 +932,10 @@
         <f t="shared" si="1"/>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (8,'payment','pay the money on CashRewards','payment',-300,1,PARSEDATETIME('01/06/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L9" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('payment','pay the money on CashRewards','payment',-300,1,PARSEDATETIME('01/06/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -931,6 +973,10 @@
         <f t="shared" si="1"/>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (9,'payment','pay the money on CashRewards','payment',300,3,PARSEDATETIME('01/06/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L10" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('payment','pay the money on CashRewards','payment',300,3,PARSEDATETIME('01/06/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -965,6 +1011,10 @@
         <f t="shared" si="1"/>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (10,'ExxonMobile','','transportation',-40,4,PARSEDATETIME('01/09/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L11" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('ExxonMobile','','transportation',-40,4,PARSEDATETIME('01/09/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1002,6 +1052,10 @@
         <f t="shared" si="1"/>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (11,'Giant','buying food','grocery',-120,3,PARSEDATETIME('01/09/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L12" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('Giant','buying food','grocery',-120,3,PARSEDATETIME('01/09/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1036,6 +1090,10 @@
         <f t="shared" si="1"/>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (12,'Retirement','','Retirement',-100,2,PARSEDATETIME('01/28/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
+      <c r="L13" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('Retirement','','Retirement',-100,2,PARSEDATETIME('01/28/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1069,6 +1127,10 @@
       <c r="K14" t="str">
         <f t="shared" si="1"/>
         <v>insert into wallet_transactions (id, store,description,category,amount,wallet,transaction_date,created_date,update_date) values (13,'Retirement','','Retirement',100,5,PARSEDATETIME('01/28/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into wallet_transactions (store,description,category,amount,wallet,transaction_date,created_date,update_date) values ('Retirement','','Retirement',100,5,PARSEDATETIME('01/28/2022','MM/dd/yyyy'),LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
     </row>
   </sheetData>
@@ -1079,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FFCC4D-CC2F-4C6E-8F0D-65B3D6FC4583}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection sqref="A1:C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,9 +1155,10 @@
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="157" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="153.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1117,8 +1180,11 @@
       <c r="G1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1141,8 +1207,12 @@
         <f>_xlfn.CONCAT($G$1,A2,",'",B2,"','",C2,"',",D2,",",E2,",",F2,");")</f>
         <v>insert into Wallets (id,name,description,balances, created_date,update_date) VALUES (1,'Checking CO','Checking acount in CO ',1000,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT($H$1,"'",B2,"','",C2,"',",D2,",",E2,",",F2,");")</f>
+        <v>insert into Wallets (name,description,balances, created_date,update_date) VALUES ('Checking CO','Checking acount in CO ',1000,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1165,8 +1235,12 @@
         <f t="shared" ref="G3:G7" si="0">_xlfn.CONCAT($G$1,A3,",'",B3,"','",C3,"',",D3,",",E3,",",F3,");")</f>
         <v>insert into Wallets (id,name,description,balances, created_date,update_date) VALUES (2,'Saving CO','Saving  account in CO',15000,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H7" si="1">_xlfn.CONCAT($H$1,"'",B3,"','",C3,"',",D3,",",E3,",",F3,");")</f>
+        <v>insert into Wallets (name,description,balances, created_date,update_date) VALUES ('Saving CO','Saving  account in CO',15000,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1189,8 +1263,12 @@
         <f t="shared" si="0"/>
         <v>insert into Wallets (id,name,description,balances, created_date,update_date) VALUES (3,'CashReward','Credit Card',-267.56,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Wallets (name,description,balances, created_date,update_date) VALUES ('CashReward','Credit Card',-267.56,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1213,8 +1291,12 @@
         <f t="shared" si="0"/>
         <v>insert into Wallets (id,name,description,balances, created_date,update_date) VALUES (4,'DoubleReward','this credit card has 5% cashback in gas purchase',-150,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Wallets (name,description,balances, created_date,update_date) VALUES ('DoubleReward','this credit card has 5% cashback in gas purchase',-150,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1237,8 +1319,12 @@
         <f t="shared" si="0"/>
         <v>insert into Wallets (id,name,description,balances, created_date,update_date) VALUES (5,'IRA','retirement account',26000,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Wallets (name,description,balances, created_date,update_date) VALUES ('IRA','retirement account',26000,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1260,6 +1346,10 @@
       <c r="G7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>insert into Wallets (id,name,description,balances, created_date,update_date) VALUES (6,'Cash','physicall cash in my pocket ',200,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into Wallets (name,description,balances, created_date,update_date) VALUES ('Cash','physicall cash in my pocket ',200,LOCALTIMESTAMP,LOCALTIMESTAMP);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>